<commit_message>
SAE-303 - Add new tab to top sports in Sarcelles dataset
</commit_message>
<xml_diff>
--- a/integration-web-s3/sae-303/datasets/crea/top-20-sports-plus-pratiques-avec-licences-par-les-sarcellois-2021.xlsx
+++ b/integration-web-s3/sae-303/datasets/crea/top-20-sports-plus-pratiques-avec-licences-par-les-sarcellois-2021.xlsx
@@ -10,13 +10,14 @@
     <sheet name="H" sheetId="1" r:id="rId1"/>
     <sheet name="F" sheetId="2" r:id="rId2"/>
     <sheet name="Tous" sheetId="3" r:id="rId3"/>
+    <sheet name="Total" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="34">
   <si>
     <t>Fédération</t>
   </si>
@@ -115,6 +116,9 @@
   </si>
   <si>
     <t>Tous</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Toutes</t>
   </si>
 </sst>
 </file>
@@ -1407,4 +1411,65 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="5.7109375" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2">
+        <v>2595</v>
+      </c>
+      <c r="D2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3">
+        <v>1161</v>
+      </c>
+      <c r="D3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>